<commit_message>
First working version of library, and first prototype of its use.
</commit_message>
<xml_diff>
--- a/Documents/TotalCodingTime.xlsx
+++ b/Documents/TotalCodingTime.xlsx
@@ -21,6 +21,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Stages</t>
+  </si>
+  <si>
+    <t>Times</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -372,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -383,28 +397,67 @@
     <col min="1" max="1" width="13.15625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1">
         <v>2.5185185185185185E-2</v>
       </c>
-      <c r="B1" s="1">
-        <f>SUM(A1:A4)</f>
-        <v>0.19721064814814815</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="2">
+      <c r="B2" s="1">
+        <f>SUM(A2:A8)</f>
+        <v>0.51555555555555554</v>
+      </c>
+      <c r="C2" s="1">
+        <f>SUM(A2:A9)</f>
+        <v>0.5552083333333333</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="2">
         <v>6.6759259259259254E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="2">
+      <c r="B3" s="1">
+        <f>SUM(A9:A9)</f>
+        <v>3.965277777777778E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="2">
         <v>6.3981481481481486E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="2">
         <v>4.1284722222222223E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="2">
+        <v>9.3368055555555551E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="2">
+        <v>0.1404050925925926</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="2">
+        <v>8.4571759259259263E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="2">
+        <v>3.965277777777778E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Redid demo and isolated it to a seperate solution.
</commit_message>
<xml_diff>
--- a/Documents/TotalCodingTime.xlsx
+++ b/Documents/TotalCodingTime.xlsx
@@ -386,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -417,8 +417,8 @@
         <v>0.51555555555555554</v>
       </c>
       <c r="C2" s="1">
-        <f>SUM(A2:A9)</f>
-        <v>0.5552083333333333</v>
+        <f>SUM(A2:A11)</f>
+        <v>0.72417824074074066</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -426,8 +426,8 @@
         <v>6.6759259259259254E-2</v>
       </c>
       <c r="B3" s="1">
-        <f>SUM(A9:A9)</f>
-        <v>3.965277777777778E-2</v>
+        <f>SUM(A9:A11)</f>
+        <v>0.2086226851851852</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -458,6 +458,16 @@
     <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2">
         <v>3.965277777777778E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="2">
+        <v>0.11260416666666667</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="2">
+        <v>5.6365740740740744E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed spawners to portals to keep with the theme, and changed head nodes to have 4 buffers instead of 2 so that it functions more smoothly and so semi-ticks work correctly.
</commit_message>
<xml_diff>
--- a/Documents/TotalCodingTime.xlsx
+++ b/Documents/TotalCodingTime.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5538"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="17268" windowHeight="5538"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -386,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -417,8 +417,8 @@
         <v>0.51555555555555554</v>
       </c>
       <c r="C2" s="1">
-        <f>SUM(A2:A11)</f>
-        <v>0.72417824074074066</v>
+        <f>SUM(A2:A12)</f>
+        <v>0.75134259259259251</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -426,8 +426,8 @@
         <v>6.6759259259259254E-2</v>
       </c>
       <c r="B3" s="1">
-        <f>SUM(A9:A11)</f>
-        <v>0.2086226851851852</v>
+        <f>SUM(A9:A12)</f>
+        <v>0.23578703703703704</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -468,6 +468,11 @@
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2">
         <v>5.6365740740740744E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="2">
+        <v>2.7164351851851853E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added serialization and multiple entry points into graphs
</commit_message>
<xml_diff>
--- a/Documents/TotalCodingTime.xlsx
+++ b/Documents/TotalCodingTime.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="17268" windowHeight="5538"/>
+    <workbookView xWindow="0" yWindow="912" windowWidth="17268" windowHeight="5538"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -386,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -417,8 +417,8 @@
         <v>0.51555555555555554</v>
       </c>
       <c r="C2" s="1">
-        <f>SUM(A2:A12)</f>
-        <v>0.75134259259259251</v>
+        <f>SUM(A2:A13)</f>
+        <v>0.78370370370370357</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -426,8 +426,8 @@
         <v>6.6759259259259254E-2</v>
       </c>
       <c r="B3" s="1">
-        <f>SUM(A9:A12)</f>
-        <v>0.23578703703703704</v>
+        <f>SUM(A9:A13)</f>
+        <v>0.26814814814814814</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -473,6 +473,11 @@
     <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2">
         <v>2.7164351851851853E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="2">
+        <v>3.2361111111111111E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Demonstrate saving models in the demo provided.
</commit_message>
<xml_diff>
--- a/Documents/TotalCodingTime.xlsx
+++ b/Documents/TotalCodingTime.xlsx
@@ -386,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -417,8 +417,8 @@
         <v>0.51555555555555554</v>
       </c>
       <c r="C2" s="1">
-        <f>SUM(A2:A13)</f>
-        <v>0.78370370370370357</v>
+        <f>SUM(A2:A14)</f>
+        <v>0.85188657407407398</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -426,8 +426,8 @@
         <v>6.6759259259259254E-2</v>
       </c>
       <c r="B3" s="1">
-        <f>SUM(A9:A13)</f>
-        <v>0.26814814814814814</v>
+        <f>SUM(A9:A14)</f>
+        <v>0.33633101851851849</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -478,6 +478,11 @@
     <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2">
         <v>3.2361111111111111E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="2">
+        <v>6.8182870370370366E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Added position variables for future graph visualization."
</commit_message>
<xml_diff>
--- a/Documents/TotalCodingTime.xlsx
+++ b/Documents/TotalCodingTime.xlsx
@@ -386,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -417,8 +417,8 @@
         <v>0.51555555555555554</v>
       </c>
       <c r="C2" s="1">
-        <f>SUM(A2:A14)</f>
-        <v>0.85188657407407398</v>
+        <f>SUM(A2:A15)</f>
+        <v>0.87211805555555544</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -426,8 +426,8 @@
         <v>6.6759259259259254E-2</v>
       </c>
       <c r="B3" s="1">
-        <f>SUM(A9:A14)</f>
-        <v>0.33633101851851849</v>
+        <f>SUM(A9:A15)</f>
+        <v>0.35656249999999995</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -483,6 +483,11 @@
     <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2">
         <v>6.8182870370370366E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="2">
+        <v>2.0231481481481482E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Altered the base library to better reflect the desired product. Began writing documentation. Added system of equations solver.
</commit_message>
<xml_diff>
--- a/Documents/TotalCodingTime.xlsx
+++ b/Documents/TotalCodingTime.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anthm\Documents\Repositories\cis598\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{070DE00E-F4C5-4FFF-AAEE-C555594E5E8B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="912" windowWidth="17268" windowHeight="5538"/>
+    <workbookView xWindow="0" yWindow="912" windowWidth="17268" windowHeight="5538" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -385,11 +386,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -414,11 +415,11 @@
       </c>
       <c r="B2" s="1">
         <f>SUM(A2:A8)</f>
-        <v>0.51555555555555554</v>
+        <v>0.51624999999999999</v>
       </c>
       <c r="C2" s="1">
-        <f>SUM(A2:A15)</f>
-        <v>0.87211805555555544</v>
+        <f>SUM(A1:A20)</f>
+        <v>1.1458333333333333</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -426,8 +427,8 @@
         <v>6.6759259259259254E-2</v>
       </c>
       <c r="B3" s="1">
-        <f>SUM(A9:A15)</f>
-        <v>0.35656249999999995</v>
+        <f>SUM(A9:A20)</f>
+        <v>0.62958333333333327</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -437,7 +438,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2">
-        <v>4.1284722222222223E-2</v>
+        <v>4.1979166666666672E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -488,6 +489,31 @@
     <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2">
         <v>2.0231481481481482E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="2">
+        <v>3.9548611111111111E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="2">
+        <v>8.621527777777778E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="2">
+        <v>8.1736111111111107E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="2">
+        <v>2.9155092592592594E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="2">
+        <v>3.636574074074074E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>